<commit_message>
Ajout d'informations et correction de bug
Ajout de nouvelles données métiers et préparation pour implémentation des résultats enrichis
Mise à jour du fichier de données et version stable avant enrichissement
</commit_message>
<xml_diff>
--- a/data/IED _ esg_calculator data.xlsx
+++ b/data/IED _ esg_calculator data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="126">
   <si>
     <t>Métier</t>
   </si>
@@ -337,7 +337,19 @@
     <t>Masters achats à l'université ou en écoles de commerce gestion</t>
   </si>
   <si>
+    <t>Mastère Spécialisé Supply Chain Durable ou Certification RSE</t>
+  </si>
+  <si>
+    <t>Durabilité &amp; Achats et Supply Chain, Cartographie des risques fournisseurs, Économie circulaire, Analyse cycle de vie, Normes ISO 20400</t>
+  </si>
+  <si>
     <t>Ailleurs : université, écoles d'agro ou d'ingénieurs</t>
+  </si>
+  <si>
+    <t>Master Écologie &amp; Biodiversité ou MSc Conservation</t>
+  </si>
+  <si>
+    <t>Préservation des écosystèmes, Mesure de la performance environnementale, Reporting biodiversité, Comptabilités multi-capitaux, Valorisation des externalités</t>
   </si>
   <si>
     <t>Croissance_Annuelle</t>
@@ -1780,13 +1792,25 @@
       <c r="B7" s="4" t="s">
         <v>106</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1812,16 +1836,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -1833,13 +1857,13 @@
         <v>0.25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3">
@@ -1851,13 +1875,13 @@
         <v>0.18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4">
@@ -1869,13 +1893,13 @@
         <v>0.15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5">
@@ -1887,13 +1911,13 @@
         <v>0.22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6">
@@ -1905,13 +1929,13 @@
         <v>0.12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7">
@@ -1923,13 +1947,13 @@
         <v>0.3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Force formulaires et sélecteurs en mode clair pour Streamlit et autres modifs mineures
Résout les problèmes d'affichage de l'interface en mode sombre en forçant un affichage clair cohérent. Modifications:
- Ajout de config.toml pour définir "base=light" comme thème par défaut
- Correction des problèmes de lisibilité des multiselect et des formulaires
- Ajout de règles CSS ciblées pour les composants qui ignoraient le paramètre base="light"
- Traduction française du placeholder pour le sélecteur de types d'entreprises
- Modifications de textes mineures
- Changement de données du fichier source
</commit_message>
<xml_diff>
--- a/data/IED _ esg_calculator data.xlsx
+++ b/data/IED _ esg_calculator data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="225">
   <si>
     <t>Métier</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Oui</t>
   </si>
   <si>
-    <t>Analyse de données, Reporting et indicateurs, Impact financier, Normes et certifications, Éthique des affaires</t>
+    <t>Analyse de données, Reporting et indicateurs, Impact financier, Réglementaire droit et juridique, Éthique des affaires</t>
   </si>
   <si>
     <t>Cabinet de conseil, Startup</t>
@@ -80,7 +80,7 @@
     <t>Data Analyst ESG</t>
   </si>
   <si>
-    <t>Analyse de données, Reporting et indicateurs, Normes et certifications, Impact financier, Vulgarisation scientifique</t>
+    <t>Analyse de données, Reporting et indicateurs, Réglementaire droit et juridique, Impact financier, Vulgarisation scientifique</t>
   </si>
   <si>
     <t>Startup, Grand groupe</t>
@@ -107,10 +107,10 @@
     <t>PME, Grand groupe</t>
   </si>
   <si>
-    <t>Juriste RSE</t>
-  </si>
-  <si>
-    <t>Conformité réglementaire, Droits humains, Normes et certifications, Éthique des affaires, Bien-être au travail</t>
+    <t>Juriste Environnement</t>
+  </si>
+  <si>
+    <t>Conformité réglementaire, Droits humains, Réglementaire droit et juridique, Éthique des affaires, Bien-être au travail</t>
   </si>
   <si>
     <t>Cabinet d'avocats, Grand groupe</t>
@@ -134,7 +134,7 @@
     <t>Conseiller en investissements financiers responsables</t>
   </si>
   <si>
-    <t>Investissement responsable, Impact financier, Éthique des affaires, Normes et certifications, Sensibilisation et pédagogie</t>
+    <t>Investissement responsable, Impact financier, Éthique des affaires, Réglementaire droit et juridique, Sensibilisation et pédagogie</t>
   </si>
   <si>
     <t>Manager sustainability risk</t>
@@ -146,7 +146,7 @@
     <t>Reporting RSE</t>
   </si>
   <si>
-    <t>Reporting et indicateurs, Communication d'impact, Normes et certifications, Analyse de données, Vulgarisation scientifique</t>
+    <t>Reporting et indicateurs, Communication d'impact, Réglementaire droit et juridique, Analyse de données, Vulgarisation scientifique</t>
   </si>
   <si>
     <t>Secteur</t>
@@ -220,6 +220,9 @@
 </t>
   </si>
   <si>
+    <t>Juriste RSE</t>
+  </si>
+  <si>
     <t>Droit</t>
   </si>
   <si>
@@ -649,16 +652,19 @@
     <t>Secteurs_Recruteurs</t>
   </si>
   <si>
+    <t>Modérée</t>
+  </si>
+  <si>
+    <t>En hausse</t>
+  </si>
+  <si>
+    <t>Finance, Asset Management, Conseil, Audit</t>
+  </si>
+  <si>
+    <t>Grandes entreprises, Industrie, Finance, Énergie</t>
+  </si>
+  <si>
     <t>Forte</t>
-  </si>
-  <si>
-    <t>En hausse</t>
-  </si>
-  <si>
-    <t>Finance, Asset Management, Conseil, Audit</t>
-  </si>
-  <si>
-    <t>Grandes entreprises, Industrie, Finance, Énergie</t>
   </si>
   <si>
     <t>PME/ETI, Collectivités, Industrie, Services</t>
@@ -1101,7 +1107,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1200,6 +1206,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="38.25"/>
+    <col customWidth="1" min="7" max="7" width="431.75"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1779,10 +1786,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>51</v>
@@ -1797,15 +1804,15 @@
         <v>35000.0</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>53</v>
@@ -1820,15 +1827,15 @@
         <v>47500.0</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>54</v>
@@ -1843,7 +1850,7 @@
         <v>65000.0</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -1851,7 +1858,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>51</v>
@@ -1866,7 +1873,7 @@
         <v>35000.0</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1874,7 +1881,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>53</v>
@@ -1889,7 +1896,7 @@
         <v>45000.0</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -1897,7 +1904,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>54</v>
@@ -1912,7 +1919,7 @@
         <v>55000.0</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -1935,7 +1942,7 @@
         <v>38500.0</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -1958,7 +1965,7 @@
         <v>55000.0</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -1981,7 +1988,7 @@
         <v>77500.0</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -2004,7 +2011,7 @@
         <v>35000.0</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -2027,7 +2034,7 @@
         <v>50000.0</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -2050,7 +2057,7 @@
         <v>75000.0</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -2073,7 +2080,7 @@
         <v>47500.0</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -2096,7 +2103,7 @@
         <v>60000.0</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -2119,7 +2126,7 @@
         <v>72500.0</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -2142,7 +2149,7 @@
         <v>33000.0</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -2165,7 +2172,7 @@
         <v>42500.0</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -2188,7 +2195,7 @@
         <v>62500.0</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44">
@@ -2373,22 +2380,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2">
@@ -2396,22 +2403,22 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3">
@@ -2419,22 +2426,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
@@ -2442,22 +2449,22 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5">
@@ -2465,22 +2472,22 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6">
@@ -2488,22 +2495,22 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7">
@@ -2511,22 +2518,22 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
@@ -2534,22 +2541,22 @@
         <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
@@ -2557,45 +2564,45 @@
         <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11">
@@ -2603,22 +2610,22 @@
         <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
@@ -2626,22 +2633,22 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13">
@@ -2649,22 +2656,22 @@
         <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14">
@@ -2672,22 +2679,22 @@
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="15">
@@ -2695,22 +2702,22 @@
         <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -2741,19 +2748,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2">
@@ -2761,19 +2768,19 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3">
@@ -2781,19 +2788,19 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4">
@@ -2801,19 +2808,19 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5">
@@ -2821,19 +2828,19 @@
         <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6">
@@ -2841,19 +2848,19 @@
         <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7">
@@ -2861,19 +2868,19 @@
         <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8">
@@ -2881,19 +2888,19 @@
         <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9">
@@ -2901,39 +2908,39 @@
         <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11">
@@ -2941,19 +2948,19 @@
         <v>33</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12">
@@ -2961,19 +2968,19 @@
         <v>35</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13">
@@ -2981,19 +2988,19 @@
         <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14">
@@ -3001,19 +3008,19 @@
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15">
@@ -3021,19 +3028,19 @@
         <v>42</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3060,16 +3067,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2">
@@ -3081,13 +3088,13 @@
         <v>0.25</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3">
@@ -3099,13 +3106,13 @@
         <v>0.18</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4">
@@ -3117,13 +3124,13 @@
         <v>0.15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5">
@@ -3135,13 +3142,13 @@
         <v>0.22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6">
@@ -3153,13 +3160,13 @@
         <v>0.12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7">
@@ -3171,13 +3178,13 @@
         <v>0.3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8">
@@ -3188,13 +3195,13 @@
         <v>0.18</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9">
@@ -3205,30 +3212,30 @@
         <v>0.16</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B10" s="4">
         <v>0.15</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11">
@@ -3239,13 +3246,13 @@
         <v>0.2</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12">
@@ -3255,14 +3262,14 @@
       <c r="B12" s="4">
         <v>0.22</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>210</v>
+      <c r="C12" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13">
@@ -3272,14 +3279,14 @@
       <c r="B13" s="4">
         <v>0.18</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>210</v>
+      <c r="C13" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="14">
@@ -3290,13 +3297,13 @@
         <v>0.2</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15">
@@ -3308,13 +3315,13 @@
         <v>0.15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>